<commit_message>
fix: Q13 and Q15 marked as 基本法 while it should be 憲法
</commit_message>
<xml_diff>
--- a/question_data.xlsx
+++ b/question_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\EMProj_QML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E7EE553-44DC-4E6F-B217-EF77857BA6A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{573D7B1B-4CBC-4B7E-8839-6C1D433267CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1142,7 +1142,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1428,7 +1428,7 @@
         <v>3</v>
       </c>
       <c r="E14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F14" t="s">
         <v>42</v>
@@ -1468,7 +1468,7 @@
         <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F16" t="s">
         <v>42</v>

</xml_diff>